<commit_message>
Existing ICDC Biobank filter fixes
</commit_message>
<xml_diff>
--- a/InputFiles/ICDC/TC02_Canine_Study_MGT01_Biobank_CSU_UCD.xlsx
+++ b/InputFiles/ICDC/TC02_Canine_Study_MGT01_Biobank_CSU_UCD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davids3\newclone\sofia0829\Commons_Automation\InputFiles\ICDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910C4A77-037F-45D1-ABB9-C0E2B3239CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{867B82E3-5FA9-442C-9209-D5028409305A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16354" yWindow="-4860" windowWidth="33120" windowHeight="18120" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -102,26 +102,6 @@
   </si>
   <si>
     <t>TC02_Canine_Study_MGT01_Biobank_CSU_UCDs_WebData.xlsx</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
-MATCH (r:registration)--&gt;(c)
-WHERE s.clinical_study_designation IN ['MGT01'] and r.registration_origin in['CSU ACTR','UCD SVM']
-WITH DISTINCT samp AS samp, c, demo, diag
-RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
-        coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(demo.breed,'') AS Breed,
-        coalesce(diag.disease_term,'') AS Diagnosis, 
-        coalesce(samp.sample_site, '') AS `Sample Site`,
-        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
-        coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
-        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
-        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
-        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
-        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
-        coalesce(samp.sample_preservation, '') AS `Sample Preservation`
-order by samp.sample_id asc
-limit 100</t>
   </si>
   <si>
     <t>MATCH (f:file)--&gt;(parent)
@@ -186,6 +166,26 @@
   coalesce(s.clinical_study_designation,'') AS `Study Code`
   order by 'File Name' asc
   limit 100</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis)
+MATCH (r:registration)--&gt;(c)
+WHERE s.clinical_study_designation IN ['MGT01'] and r.registration_origin in['CSU ACTR','UCD SVM']
+WITH DISTINCT samp AS samp, c, demo, diag
+RETURN  coalesce(samp.sample_id, '') AS `Sample ID`,
+        coalesce(c.case_id, '') AS `Case ID`,
+        coalesce(demo.breed,'') AS Breed,
+        coalesce(diag.disease_term,'') AS Diagnosis,
+        coalesce(samp.sample_site, '') AS `Sample Site`,
+        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
+        replace(coalesce(samp.specific_sample_pathology, ''), "  ", " ") AS `Pathology/Morphology`,
+        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
+        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
+        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
+        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
+        coalesce(samp.sample_preservation, '') AS `Sample Preservation`
+order by samp.sample_id asc
+limit 100</t>
   </si>
 </sst>
 </file>
@@ -569,19 +569,19 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="87.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="75.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="70.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="28.5546875" style="1" customWidth="1"/>
-    <col min="6" max="10" width="9.109375" style="1"/>
-    <col min="11" max="11" width="21.33203125" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="24.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="87.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="75.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="70.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" style="1" customWidth="1"/>
+    <col min="6" max="10" width="9.140625" style="1"/>
+    <col min="11" max="11" width="21.28515625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -598,7 +598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="409.6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -615,12 +615,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="360" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="393.75" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>10</v>
@@ -632,12 +632,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>10</v>
@@ -649,12 +649,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="409.6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>

</xml_diff>